<commit_message>
Add `Animals` XLS sheet
Ludovic updated it to the newest version
</commit_message>
<xml_diff>
--- a/Animals.xlsx
+++ b/Animals.xlsx
@@ -1,33 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26129"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Documents\Hearts-Melly\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C30688B-C3FA-4051-A053-81659E353D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="255" windowWidth="11340" windowHeight="5325"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26100" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="6">
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>M</t>
   </si>
   <si>
     <t>EPI</t>
   </si>
   <si>
     <t>V+P</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
   <si>
     <t>tachosil only</t>
@@ -39,8 +58,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,7 +106,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -95,14 +114,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -140,9 +162,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,9 +197,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,9 +249,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -385,21 +441,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="1">
         <v>60</v>
       </c>
@@ -407,16 +463,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="1">
         <v>61</v>
       </c>
@@ -424,16 +480,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75">
       <c r="A3" s="1">
         <v>62</v>
       </c>
@@ -441,7 +497,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -450,7 +506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="1">
         <v>63</v>
       </c>
@@ -458,7 +514,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -467,15 +523,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="1">
         <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
@@ -484,15 +540,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="1">
         <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>4</v>
@@ -501,32 +557,32 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="1">
         <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="E7" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75">
       <c r="A8" s="1">
         <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>0</v>
@@ -535,32 +591,32 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75">
       <c r="A9" s="1">
         <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="E9" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.75">
       <c r="A10" s="1">
         <v>69</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>0</v>
@@ -569,15 +625,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.75">
       <c r="A11" s="1">
         <v>70</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>4</v>
@@ -586,15 +642,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.75">
       <c r="A12" s="1">
         <v>71</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>4</v>
@@ -603,15 +659,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15.75">
       <c r="A13" s="1">
         <v>79</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>0</v>
@@ -620,49 +676,49 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.75">
       <c r="A14" s="1">
         <v>80</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="E14" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15.75">
       <c r="A15" s="1">
         <v>81</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="E15" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15.75">
       <c r="A16" s="1">
         <v>82</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>5</v>
@@ -671,15 +727,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.75">
       <c r="A17" s="1">
         <v>83</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>5</v>
@@ -688,21 +744,123 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.75">
       <c r="A18" s="1">
         <v>84</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="3">
         <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75">
+      <c r="A19" s="1">
+        <v>85</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75">
+      <c r="A20" s="1">
+        <v>86</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75">
+      <c r="A21" s="1">
+        <v>87</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75">
+      <c r="A22" s="1">
+        <v>88</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75">
+      <c r="A23" s="1">
+        <v>89</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75">
+      <c r="A24" s="1">
+        <v>90</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -711,24 +869,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>